<commit_message>
agregado de 6A instrumentacion y 7A- comp Aer, valoracion media
</commit_message>
<xml_diff>
--- a/inasistencias-6A-InstrumentalYsistElect/Alumnos-6A-InstrumentalYsistElect.xlsx
+++ b/inasistencias-6A-InstrumentalYsistElect/Alumnos-6A-InstrumentalYsistElect.xlsx
@@ -13,6 +13,11 @@
     <sheet name="1-volt Amp" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="2-volt multi" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="3-amp multi" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="1-Recup" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="2-recup" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="3-recup" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="4-Thevenin- positivos" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="positivos" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="284">
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
@@ -281,18 +286,27 @@
     <t xml:space="preserve">1-volt y amp</t>
   </si>
   <si>
+    <t xml:space="preserve">Recup</t>
+  </si>
+  <si>
     <t xml:space="preserve">2- vol multi</t>
   </si>
   <si>
     <t xml:space="preserve">3-amp multi</t>
   </si>
   <si>
-    <t xml:space="preserve">4-Thev y Nor</t>
-  </si>
-  <si>
     <t xml:space="preserve">positivos</t>
   </si>
   <si>
+    <t xml:space="preserve">3+positivos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">promedio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valoracion</t>
+  </si>
+  <si>
     <t xml:space="preserve">Finalizado</t>
   </si>
   <si>
@@ -302,9 +316,6 @@
     <t xml:space="preserve">Calificación/10,00</t>
   </si>
   <si>
-    <t xml:space="preserve">promedio</t>
-  </si>
-  <si>
     <t xml:space="preserve">segundo</t>
   </si>
   <si>
@@ -735,15 +746,151 @@
   </si>
   <si>
     <t xml:space="preserve">27 de abril de 2025  20:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total notas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calificación/9,00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P. 1 /1,00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P. 2 /1,00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P. 3 /1,00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P. 4 /1,00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P. 5 /1,00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P. 6 /1,00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P. 7 /1,00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P. 8 /1,00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P. 9 /1,00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 de abril de 2025  20:16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 minutos 14 segundos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 de mayo de 2025  23:18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 minutos 5 segundos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 de mayo de 2025  14:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34 minutos 41 segundos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 de mayo de 2025  23:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 minutos 42 segundos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 de abril de 2025  21:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 minutos 4 segundos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 de mayo de 2025  13:12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 minutos 3 segundos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 de mayo de 2025  14:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 minutos 3 segundos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 de mayo de 2025  23:44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 minutos 55 segundos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P. 1 /1,67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P. 2 /8,33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 de abril de 2025  19:59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 minutos 12 segundos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 de abril de 2025  19:51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 minutos 18 segundos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 de abril de 2025  19:55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 minutos 25 segundos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 de abril de 2025  19:57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 minutos 33 segundos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 minutos 42 segundos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 de abril de 2025  19:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 minutos 40 segundos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 de abril de 2025  19:56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 minutos 22 segundos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thevenin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -769,12 +916,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -811,7 +964,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -824,6 +977,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -833,6 +994,98 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="0"/>
+        <b val="1"/>
+        <color rgb="FFFFFFFF"/>
+        <sz val="12"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF232629"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -843,11 +1096,11 @@
   </sheetPr>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.6"/>
@@ -1330,24 +1583,555 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H28"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.6"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="n">
+        <v>45736</v>
+      </c>
+      <c r="D1" s="2" t="n">
+        <v>45736</v>
+      </c>
+      <c r="E1" s="2" t="n">
+        <v>-620088</v>
+      </c>
+      <c r="F1" s="2" t="n">
+        <v>45757</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <f aca="false">SUM(C2:G2)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <f aca="false">SUM(C3:G3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <f aca="false">SUM(C4:G4)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <f aca="false">SUM(C5:G5)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <f aca="false">SUM(C6:G6)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <f aca="false">SUM(C7:G7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <f aca="false">SUM(C8:G8)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <f aca="false">SUM(C9:G9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <f aca="false">SUM(C10:G10)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <f aca="false">SUM(C11:G11)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <f aca="false">SUM(C12:G12)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <f aca="false">SUM(C13:G13)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <f aca="false">SUM(C14:G14)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <f aca="false">SUM(C15:G15)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <f aca="false">SUM(C16:G16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <f aca="false">SUM(C17:G17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <f aca="false">SUM(C18:G18)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <f aca="false">SUM(C19:G19)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <f aca="false">SUM(C20:G20)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <f aca="false">SUM(C21:G21)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <f aca="false">SUM(C22:G22)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <f aca="false">SUM(C23:G23)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <f aca="false">SUM(C24:G24)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <f aca="false">SUM(C25:G25)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <f aca="false">SUM(C26:G26)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <f aca="false">SUM(C27:G27)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <f aca="false">COUNTIF(C2:C27,"&gt;0")</f>
+        <v>19</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <f aca="false">COUNTIF(D2:D27,"&gt;0")</f>
+        <v>11</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <f aca="false">COUNTIF(E2:E27,"&gt;0")</f>
+        <v>9</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <f aca="false">COUNTIF(F2:F27,"&gt;0")</f>
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M28" activeCellId="0" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1367,10 +2151,25 @@
         <v>86</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" s="0" t="s">
         <v>88</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1383,8 +2182,26 @@
       <c r="C2" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="E2" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <f aca="false">G2+I2/2</f>
+        <v>6.5</v>
+      </c>
+      <c r="K2" s="3" t="n">
+        <f aca="false">ROUND(AVERAGE(C2,E2,J2),0)</f>
+        <v>8</v>
+      </c>
+      <c r="L2" s="0" t="str">
+        <f aca="false">IF(K2&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1397,8 +2214,26 @@
       <c r="C3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <v>1</v>
+      <c r="E3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <f aca="false">G3+I3/2</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="3" t="n">
+        <f aca="false">ROUND(AVERAGE(C3,E3,J3),0)</f>
+        <v>1</v>
+      </c>
+      <c r="L3" s="0" t="str">
+        <f aca="false">IF(K3&lt;7,"TEP","TEA")</f>
+        <v>TEP</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1411,8 +2246,26 @@
       <c r="C4" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="E4" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <f aca="false">G4+I4/2</f>
+        <v>8</v>
+      </c>
+      <c r="K4" s="3" t="n">
+        <f aca="false">ROUND(AVERAGE(C4,E4,J4),0)</f>
+        <v>9</v>
+      </c>
+      <c r="L4" s="0" t="str">
+        <f aca="false">IF(K4&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1425,8 +2278,26 @@
       <c r="C5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <v>1</v>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <f aca="false">G5+I5/2</f>
+        <v>6</v>
+      </c>
+      <c r="K5" s="3" t="n">
+        <f aca="false">ROUND(AVERAGE(C5,E5,J5),0)</f>
+        <v>3</v>
+      </c>
+      <c r="L5" s="0" t="str">
+        <f aca="false">IF(K5&lt;7,"TEP","TEA")</f>
+        <v>TEP</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1439,8 +2310,26 @@
       <c r="C6" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <v>1</v>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <f aca="false">G6+I6/2</f>
+        <v>2.5</v>
+      </c>
+      <c r="K6" s="3" t="n">
+        <f aca="false">ROUND(AVERAGE(C6,E6,J6),0)</f>
+        <v>2</v>
+      </c>
+      <c r="L6" s="0" t="str">
+        <f aca="false">IF(K6&lt;7,"TEP","TEA")</f>
+        <v>TEP</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1453,8 +2342,26 @@
       <c r="C7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D7" s="0" t="n">
-        <v>1</v>
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <f aca="false">G7+I7/2</f>
+        <v>1</v>
+      </c>
+      <c r="K7" s="3" t="n">
+        <f aca="false">ROUND(AVERAGE(C7,E7,J7),0)</f>
+        <v>1</v>
+      </c>
+      <c r="L7" s="0" t="str">
+        <f aca="false">IF(K7&lt;7,"TEP","TEA")</f>
+        <v>TEP</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1467,8 +2374,29 @@
       <c r="C8" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="E8" s="0" t="n">
         <v>7</v>
+      </c>
+      <c r="G8" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>45784</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <f aca="false">G8+I8/2</f>
+        <v>9.5</v>
+      </c>
+      <c r="K8" s="3" t="n">
+        <f aca="false">ROUND(AVERAGE(C8,E8,J8),0)</f>
+        <v>8</v>
+      </c>
+      <c r="L8" s="0" t="str">
+        <f aca="false">IF(K8&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1481,8 +2409,26 @@
       <c r="C9" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="E9" s="0" t="n">
         <v>3</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <f aca="false">G9+I9/2</f>
+        <v>1</v>
+      </c>
+      <c r="K9" s="3" t="n">
+        <f aca="false">ROUND(AVERAGE(C9,E9,J9),0)</f>
+        <v>4</v>
+      </c>
+      <c r="L9" s="0" t="str">
+        <f aca="false">IF(K9&lt;7,"TEP","TEA")</f>
+        <v>TEP</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1495,8 +2441,26 @@
       <c r="C10" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="E10" s="0" t="n">
         <v>8</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <f aca="false">G10+I10/2</f>
+        <v>15</v>
+      </c>
+      <c r="K10" s="3" t="n">
+        <f aca="false">ROUND(AVERAGE(C10,E10,J10),0)</f>
+        <v>10</v>
+      </c>
+      <c r="L10" s="0" t="str">
+        <f aca="false">IF(K10&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1509,8 +2473,32 @@
       <c r="C11" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="D11" s="0" t="n">
-        <v>1</v>
+      <c r="E11" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>45784</v>
+      </c>
+      <c r="G11" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>45784</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <f aca="false">G11+I11/2</f>
+        <v>6.5</v>
+      </c>
+      <c r="K11" s="3" t="n">
+        <f aca="false">ROUND(AVERAGE(C11,E11,J11),0)</f>
+        <v>7</v>
+      </c>
+      <c r="L11" s="0" t="str">
+        <f aca="false">IF(K11&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1523,8 +2511,26 @@
       <c r="C12" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="E12" s="0" t="n">
         <v>7</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <f aca="false">G12+I12/2</f>
+        <v>2.5</v>
+      </c>
+      <c r="K12" s="3" t="n">
+        <f aca="false">ROUND(AVERAGE(C12,E12,J12),0)</f>
+        <v>5</v>
+      </c>
+      <c r="L12" s="0" t="str">
+        <f aca="false">IF(K12&lt;7,"TEP","TEA")</f>
+        <v>TEP</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1534,11 +2540,38 @@
       <c r="B13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>1</v>
+      <c r="C13" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>45782</v>
+      </c>
+      <c r="E13" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>45782</v>
+      </c>
+      <c r="G13" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>45782</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <f aca="false">G13+I13/2</f>
+        <v>5.5</v>
+      </c>
+      <c r="K13" s="3" t="n">
+        <f aca="false">ROUND(AVERAGE(C13,E13,J13),0)</f>
+        <v>5</v>
+      </c>
+      <c r="L13" s="0" t="str">
+        <f aca="false">IF(K13&lt;7,"TEP","TEA")</f>
+        <v>TEP</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1551,8 +2584,26 @@
       <c r="C14" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="D14" s="0" t="n">
-        <v>9</v>
+      <c r="E14" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <f aca="false">G14+I14/2</f>
+        <v>14</v>
+      </c>
+      <c r="K14" s="3" t="n">
+        <f aca="false">ROUND(AVERAGE(C14,E14,J14),0)</f>
+        <v>11</v>
+      </c>
+      <c r="L14" s="0" t="str">
+        <f aca="false">IF(K14&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1565,8 +2616,26 @@
       <c r="C15" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="E15" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <f aca="false">G15+I15/2</f>
+        <v>10</v>
+      </c>
+      <c r="K15" s="3" t="n">
+        <f aca="false">ROUND(AVERAGE(C15,E15,J15),0)</f>
+        <v>10</v>
+      </c>
+      <c r="L15" s="0" t="str">
+        <f aca="false">IF(K15&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1579,8 +2648,26 @@
       <c r="C16" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="E16" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <f aca="false">G16+I16/2</f>
+        <v>1</v>
+      </c>
+      <c r="K16" s="3" t="n">
+        <f aca="false">ROUND(AVERAGE(C16,E16,J16),0)</f>
+        <v>5</v>
+      </c>
+      <c r="L16" s="0" t="str">
+        <f aca="false">IF(K16&lt;7,"TEP","TEA")</f>
+        <v>TEP</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1593,8 +2680,27 @@
       <c r="C17" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="D17" s="0" t="n">
-        <v>1</v>
+      <c r="E17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <f aca="false">MAX(F17,E17)</f>
+        <v>1</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <f aca="false">G17+I17/2</f>
+        <v>1</v>
+      </c>
+      <c r="K17" s="3" t="n">
+        <f aca="false">ROUND(AVERAGE(C17,E17,J17),0)</f>
+        <v>3</v>
+      </c>
+      <c r="L17" s="0" t="str">
+        <f aca="false">IF(K17&lt;7,"TEP","TEA")</f>
+        <v>TEP</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1607,8 +2713,26 @@
       <c r="C18" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="D18" s="0" t="n">
-        <v>1</v>
+      <c r="E18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <f aca="false">G18+I18/2</f>
+        <v>10</v>
+      </c>
+      <c r="K18" s="3" t="n">
+        <f aca="false">ROUND(AVERAGE(C18,E18,J18),0)</f>
+        <v>6</v>
+      </c>
+      <c r="L18" s="0" t="str">
+        <f aca="false">IF(K18&lt;7,"TEP","TEA")</f>
+        <v>TEP</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1621,8 +2745,26 @@
       <c r="C19" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="D19" s="0" t="n">
-        <v>1</v>
+      <c r="E19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <f aca="false">G19+I19/2</f>
+        <v>10</v>
+      </c>
+      <c r="K19" s="3" t="n">
+        <f aca="false">ROUND(AVERAGE(C19,E19,J19),0)</f>
+        <v>6</v>
+      </c>
+      <c r="L19" s="0" t="str">
+        <f aca="false">IF(K19&lt;7,"TEP","TEA")</f>
+        <v>TEP</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1635,8 +2777,29 @@
       <c r="C20" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="D20" s="0" t="n">
-        <v>5</v>
+      <c r="E20" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>45751</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <f aca="false">G20+I20/2</f>
+        <v>11.5</v>
+      </c>
+      <c r="K20" s="3" t="n">
+        <f aca="false">ROUND(AVERAGE(C20,E20,J20),0)</f>
+        <v>10</v>
+      </c>
+      <c r="L20" s="0" t="str">
+        <f aca="false">IF(K20&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1649,8 +2812,26 @@
       <c r="C21" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D21" s="0" t="n">
-        <v>1</v>
+      <c r="E21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <f aca="false">G21+I21/2</f>
+        <v>2</v>
+      </c>
+      <c r="K21" s="3" t="n">
+        <f aca="false">ROUND(AVERAGE(C21,E21,J21),0)</f>
+        <v>1</v>
+      </c>
+      <c r="L21" s="0" t="str">
+        <f aca="false">IF(K21&lt;7,"TEP","TEA")</f>
+        <v>TEP</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1663,8 +2844,26 @@
       <c r="C22" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="E22" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <f aca="false">G22+I22/2</f>
+        <v>9.5</v>
+      </c>
+      <c r="K22" s="3" t="n">
+        <f aca="false">ROUND(AVERAGE(C22,E22,J22),0)</f>
+        <v>10</v>
+      </c>
+      <c r="L22" s="0" t="str">
+        <f aca="false">IF(K22&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1677,8 +2876,27 @@
       <c r="C23" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="E23" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <f aca="false">MAX(F24,E24)</f>
+        <v>10</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <f aca="false">G23+I23/2</f>
+        <v>13</v>
+      </c>
+      <c r="K23" s="3" t="n">
+        <f aca="false">ROUND(AVERAGE(C23,E23,J23),0)</f>
+        <v>11</v>
+      </c>
+      <c r="L23" s="0" t="str">
+        <f aca="false">IF(K23&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1691,8 +2909,26 @@
       <c r="C24" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="E24" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="J24" s="0" t="n">
+        <f aca="false">G24+I24/2</f>
+        <v>14.5</v>
+      </c>
+      <c r="K24" s="3" t="n">
+        <f aca="false">ROUND(AVERAGE(C24,E24,J24),0)</f>
+        <v>11</v>
+      </c>
+      <c r="L24" s="0" t="str">
+        <f aca="false">IF(K24&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1705,8 +2941,26 @@
       <c r="C25" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="E25" s="0" t="n">
         <v>7</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="J25" s="0" t="n">
+        <f aca="false">G25+I25/2</f>
+        <v>24.5</v>
+      </c>
+      <c r="K25" s="3" t="n">
+        <f aca="false">ROUND(AVERAGE(C25,E25,J25),0)</f>
+        <v>14</v>
+      </c>
+      <c r="L25" s="0" t="str">
+        <f aca="false">IF(K25&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1719,8 +2973,26 @@
       <c r="C26" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="E26" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <f aca="false">G26+I26/2</f>
+        <v>20</v>
+      </c>
+      <c r="K26" s="3" t="n">
+        <f aca="false">ROUND(AVERAGE(C26,E26,J26),0)</f>
+        <v>13</v>
+      </c>
+      <c r="L26" s="0" t="str">
+        <f aca="false">IF(K26&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1733,46 +3005,39 @@
       <c r="C27" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="E27" s="0" t="n">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="G27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <f aca="false">G27+I27/2</f>
+        <v>2.5</v>
+      </c>
+      <c r="K27" s="3" t="n">
+        <f aca="false">ROUND(AVERAGE(C27,E27,J27),0)</f>
+        <v>5</v>
+      </c>
+      <c r="L27" s="0" t="str">
+        <f aca="false">IF(K27&lt;7,"TEP","TEA")</f>
+        <v>TEP</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="K2:K27">
+    <cfRule type="cellIs" priority="2" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L27">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"TEP"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1790,11 +3055,11 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.83"/>
@@ -1806,22 +3071,22 @@
         <v>1</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E1" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="F1" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>92</v>
-      </c>
       <c r="H1" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1835,10 +3100,10 @@
         <v>4</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>8</v>
@@ -1858,10 +3123,10 @@
         <v>8</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>1</v>
@@ -1881,10 +3146,10 @@
         <v>11</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>9</v>
@@ -1918,10 +3183,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>5</v>
@@ -1943,10 +3208,10 @@
         <v>18</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>1</v>
@@ -1963,10 +3228,10 @@
         <v>21</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>1</v>
@@ -1986,10 +3251,10 @@
         <v>24</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>9</v>
@@ -2011,10 +3276,10 @@
         <v>24</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>8</v>
@@ -2025,10 +3290,10 @@
         <v>24</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>8</v>
@@ -2039,10 +3304,10 @@
         <v>24</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>3</v>
@@ -2059,10 +3324,10 @@
         <v>27</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>9</v>
@@ -2082,10 +3347,10 @@
         <v>30</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>7</v>
@@ -2105,10 +3370,10 @@
         <v>33</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>8</v>
@@ -2128,10 +3393,10 @@
         <v>36</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>8</v>
@@ -2153,10 +3418,10 @@
         <v>36</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>4</v>
@@ -2173,10 +3438,10 @@
         <v>39</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>1</v>
@@ -2196,10 +3461,10 @@
         <v>42</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>10</v>
@@ -2221,10 +3486,10 @@
         <v>42</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>9</v>
@@ -2235,10 +3500,10 @@
         <v>42</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>8</v>
@@ -2249,10 +3514,10 @@
         <v>42</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>3</v>
@@ -2269,10 +3534,10 @@
         <v>45</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>9</v>
@@ -2292,10 +3557,10 @@
         <v>48</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>9</v>
@@ -2315,10 +3580,10 @@
         <v>51</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>9</v>
@@ -2340,10 +3605,10 @@
         <v>51</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>4</v>
@@ -2360,10 +3625,10 @@
         <v>54</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>7</v>
@@ -2383,10 +3648,10 @@
         <v>57</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>8</v>
@@ -2408,10 +3673,10 @@
         <v>57</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>5</v>
@@ -2428,10 +3693,10 @@
         <v>60</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>10</v>
@@ -2451,10 +3716,10 @@
         <v>63</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F31" s="0" t="n">
         <v>1</v>
@@ -2474,10 +3739,10 @@
         <v>66</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F32" s="0" t="n">
         <v>9</v>
@@ -2497,10 +3762,10 @@
         <v>69</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F33" s="0" t="n">
         <v>9</v>
@@ -2520,10 +3785,10 @@
         <v>72</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F34" s="0" t="n">
         <v>9</v>
@@ -2543,10 +3808,10 @@
         <v>75</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F35" s="0" t="n">
         <v>9</v>
@@ -2568,10 +3833,10 @@
         <v>75</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F36" s="0" t="n">
         <v>9</v>
@@ -2582,10 +3847,10 @@
         <v>75</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="F37" s="0" t="n">
         <v>9</v>
@@ -2602,10 +3867,10 @@
         <v>78</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="F38" s="0" t="n">
         <v>8</v>
@@ -2625,10 +3890,10 @@
         <v>81</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="F39" s="0" t="n">
         <v>6</v>
@@ -2657,11 +3922,11 @@
   </sheetPr>
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.38671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="18.83"/>
   </cols>
@@ -2671,22 +3936,22 @@
         <v>1</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E1" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="F1" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>92</v>
-      </c>
       <c r="H1" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2700,10 +3965,10 @@
         <v>4</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>10</v>
@@ -2737,10 +4002,10 @@
         <v>11</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>10</v>
@@ -2802,10 +4067,10 @@
         <v>24</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>10</v>
@@ -2827,10 +4092,10 @@
         <v>24</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>7</v>
@@ -2841,10 +4106,10 @@
         <v>24</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>7</v>
@@ -2855,10 +4120,10 @@
         <v>24</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>6</v>
@@ -2869,10 +4134,10 @@
         <v>24</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>4</v>
@@ -2903,10 +4168,10 @@
         <v>30</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>8</v>
@@ -2940,10 +4205,10 @@
         <v>36</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>7</v>
@@ -2977,10 +4242,10 @@
         <v>42</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>9</v>
@@ -3000,10 +4265,10 @@
         <v>45</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>10</v>
@@ -3023,10 +4288,10 @@
         <v>48</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>5</v>
@@ -3046,10 +4311,10 @@
         <v>51</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>1</v>
@@ -3097,10 +4362,10 @@
         <v>60</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>5</v>
@@ -3120,10 +4385,10 @@
         <v>63</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>1</v>
@@ -3143,10 +4408,10 @@
         <v>66</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>10</v>
@@ -3166,10 +4431,10 @@
         <v>69</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>10</v>
@@ -3189,10 +4454,10 @@
         <v>72</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>10</v>
@@ -3212,10 +4477,10 @@
         <v>75</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>10</v>
@@ -3237,10 +4502,10 @@
         <v>75</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>1</v>
@@ -3257,10 +4522,10 @@
         <v>78</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="F31" s="0" t="n">
         <v>10</v>
@@ -3280,10 +4545,10 @@
         <v>81</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="F32" s="0" t="n">
         <v>7</v>
@@ -3323,11 +4588,11 @@
   </sheetPr>
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J26" activeCellId="0" sqref="J26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I29" activeCellId="0" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.38671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="18.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.95"/>
@@ -3339,22 +4604,22 @@
         <v>1</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E1" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="F1" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>92</v>
-      </c>
       <c r="H1" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3368,10 +4633,10 @@
         <v>4</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>5</v>
@@ -3405,10 +4670,10 @@
         <v>11</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>6</v>
@@ -3428,10 +4693,10 @@
         <v>14</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>3</v>
@@ -3507,10 +4772,10 @@
         <v>30</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>9</v>
@@ -3572,10 +4837,10 @@
         <v>42</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>9</v>
@@ -3595,10 +4860,10 @@
         <v>45</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>6</v>
@@ -3632,10 +4897,10 @@
         <v>51</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>10</v>
@@ -3657,10 +4922,10 @@
         <v>51</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>6</v>
@@ -3677,10 +4942,10 @@
         <v>54</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>7</v>
@@ -3700,10 +4965,10 @@
         <v>57</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>6</v>
@@ -3723,10 +4988,10 @@
         <v>60</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>10</v>
@@ -3760,10 +5025,10 @@
         <v>66</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>8</v>
@@ -3783,10 +5048,10 @@
         <v>69</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>10</v>
@@ -3808,10 +5073,10 @@
         <v>69</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>9</v>
@@ -3828,10 +5093,10 @@
         <v>72</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>10</v>
@@ -3851,10 +5116,10 @@
         <v>75</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>9</v>
@@ -3874,10 +5139,10 @@
         <v>78</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>10</v>
@@ -3900,7 +5165,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H30" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <f aca="false">COUNTIF(I2:I29,"&gt;0")</f>
+        <v>26</v>
+      </c>
+    </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3917,4 +5190,764 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.19"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.19"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.11"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <f aca="false">ROUND(D2,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <f aca="false">ROUND(D3,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <f aca="false">ROUND(D4,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <f aca="false">ROUND(D5,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <f aca="false">ROUND(D6,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <f aca="false">ROUND(D7,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>8.33</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <f aca="false">ROUND(D8,0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <f aca="false">ROUND(D9,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
instrumental de 5to actualizacion
</commit_message>
<xml_diff>
--- a/inasistencias-6A-InstrumentalYsistElect/Alumnos-6A-InstrumentalYsistElect.xlsx
+++ b/inasistencias-6A-InstrumentalYsistElect/Alumnos-6A-InstrumentalYsistElect.xlsx
@@ -964,7 +964,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -974,6 +974,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -994,7 +998,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="1">
     <dxf>
       <font>
         <name val="Calibri"/>
@@ -1007,21 +1011,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFCC0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF232629"/>
-          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1100,7 +1089,7 @@
       <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.6"/>
@@ -1594,7 +1583,7 @@
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.6"/>
@@ -2122,10 +2111,10 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M28" activeCellId="0" sqref="M28"/>
+      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.40234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.57"/>
@@ -2199,7 +2188,7 @@
         <f aca="false">ROUND(AVERAGE(C2,E2,J2),0)</f>
         <v>8</v>
       </c>
-      <c r="L2" s="0" t="str">
+      <c r="L2" s="4" t="str">
         <f aca="false">IF(K2&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -2231,7 +2220,7 @@
         <f aca="false">ROUND(AVERAGE(C3,E3,J3),0)</f>
         <v>1</v>
       </c>
-      <c r="L3" s="0" t="str">
+      <c r="L3" s="4" t="str">
         <f aca="false">IF(K3&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -2263,7 +2252,7 @@
         <f aca="false">ROUND(AVERAGE(C4,E4,J4),0)</f>
         <v>9</v>
       </c>
-      <c r="L4" s="0" t="str">
+      <c r="L4" s="4" t="str">
         <f aca="false">IF(K4&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -2295,7 +2284,7 @@
         <f aca="false">ROUND(AVERAGE(C5,E5,J5),0)</f>
         <v>3</v>
       </c>
-      <c r="L5" s="0" t="str">
+      <c r="L5" s="4" t="str">
         <f aca="false">IF(K5&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -2327,7 +2316,7 @@
         <f aca="false">ROUND(AVERAGE(C6,E6,J6),0)</f>
         <v>2</v>
       </c>
-      <c r="L6" s="0" t="str">
+      <c r="L6" s="4" t="str">
         <f aca="false">IF(K6&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -2359,7 +2348,7 @@
         <f aca="false">ROUND(AVERAGE(C7,E7,J7),0)</f>
         <v>1</v>
       </c>
-      <c r="L7" s="0" t="str">
+      <c r="L7" s="4" t="str">
         <f aca="false">IF(K7&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -2377,7 +2366,7 @@
       <c r="E8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="G8" s="4" t="n">
+      <c r="G8" s="5" t="n">
         <v>6</v>
       </c>
       <c r="H8" s="2" t="n">
@@ -2394,7 +2383,7 @@
         <f aca="false">ROUND(AVERAGE(C8,E8,J8),0)</f>
         <v>8</v>
       </c>
-      <c r="L8" s="0" t="str">
+      <c r="L8" s="4" t="str">
         <f aca="false">IF(K8&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -2426,7 +2415,7 @@
         <f aca="false">ROUND(AVERAGE(C9,E9,J9),0)</f>
         <v>4</v>
       </c>
-      <c r="L9" s="0" t="str">
+      <c r="L9" s="4" t="str">
         <f aca="false">IF(K9&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -2458,7 +2447,7 @@
         <f aca="false">ROUND(AVERAGE(C10,E10,J10),0)</f>
         <v>10</v>
       </c>
-      <c r="L10" s="0" t="str">
+      <c r="L10" s="4" t="str">
         <f aca="false">IF(K10&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -2473,13 +2462,13 @@
       <c r="C11" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="E11" s="4" t="n">
+      <c r="E11" s="5" t="n">
         <v>7</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>45784</v>
       </c>
-      <c r="G11" s="4" t="n">
+      <c r="G11" s="5" t="n">
         <v>6</v>
       </c>
       <c r="H11" s="2" t="n">
@@ -2496,7 +2485,7 @@
         <f aca="false">ROUND(AVERAGE(C11,E11,J11),0)</f>
         <v>7</v>
       </c>
-      <c r="L11" s="0" t="str">
+      <c r="L11" s="4" t="str">
         <f aca="false">IF(K11&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -2528,7 +2517,7 @@
         <f aca="false">ROUND(AVERAGE(C12,E12,J12),0)</f>
         <v>5</v>
       </c>
-      <c r="L12" s="0" t="str">
+      <c r="L12" s="4" t="str">
         <f aca="false">IF(K12&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -2540,19 +2529,19 @@
       <c r="B13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="4" t="n">
+      <c r="C13" s="5" t="n">
         <v>6</v>
       </c>
       <c r="D13" s="2" t="n">
         <v>45782</v>
       </c>
-      <c r="E13" s="4" t="n">
+      <c r="E13" s="5" t="n">
         <v>4</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>45782</v>
       </c>
-      <c r="G13" s="4" t="n">
+      <c r="G13" s="5" t="n">
         <v>3</v>
       </c>
       <c r="H13" s="2" t="n">
@@ -2569,7 +2558,7 @@
         <f aca="false">ROUND(AVERAGE(C13,E13,J13),0)</f>
         <v>5</v>
       </c>
-      <c r="L13" s="0" t="str">
+      <c r="L13" s="4" t="str">
         <f aca="false">IF(K13&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -2601,7 +2590,7 @@
         <f aca="false">ROUND(AVERAGE(C14,E14,J14),0)</f>
         <v>11</v>
       </c>
-      <c r="L14" s="0" t="str">
+      <c r="L14" s="4" t="str">
         <f aca="false">IF(K14&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -2633,7 +2622,7 @@
         <f aca="false">ROUND(AVERAGE(C15,E15,J15),0)</f>
         <v>10</v>
       </c>
-      <c r="L15" s="0" t="str">
+      <c r="L15" s="4" t="str">
         <f aca="false">IF(K15&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -2665,7 +2654,7 @@
         <f aca="false">ROUND(AVERAGE(C16,E16,J16),0)</f>
         <v>5</v>
       </c>
-      <c r="L16" s="0" t="str">
+      <c r="L16" s="4" t="str">
         <f aca="false">IF(K16&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -2698,7 +2687,7 @@
         <f aca="false">ROUND(AVERAGE(C17,E17,J17),0)</f>
         <v>3</v>
       </c>
-      <c r="L17" s="0" t="str">
+      <c r="L17" s="4" t="str">
         <f aca="false">IF(K17&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -2730,7 +2719,7 @@
         <f aca="false">ROUND(AVERAGE(C18,E18,J18),0)</f>
         <v>6</v>
       </c>
-      <c r="L18" s="0" t="str">
+      <c r="L18" s="4" t="str">
         <f aca="false">IF(K18&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -2762,7 +2751,7 @@
         <f aca="false">ROUND(AVERAGE(C19,E19,J19),0)</f>
         <v>6</v>
       </c>
-      <c r="L19" s="0" t="str">
+      <c r="L19" s="4" t="str">
         <f aca="false">IF(K19&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -2777,7 +2766,7 @@
       <c r="C20" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="E20" s="4" t="n">
+      <c r="E20" s="5" t="n">
         <v>9</v>
       </c>
       <c r="F20" s="2" t="n">
@@ -2797,7 +2786,7 @@
         <f aca="false">ROUND(AVERAGE(C20,E20,J20),0)</f>
         <v>10</v>
       </c>
-      <c r="L20" s="0" t="str">
+      <c r="L20" s="4" t="str">
         <f aca="false">IF(K20&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -2829,7 +2818,7 @@
         <f aca="false">ROUND(AVERAGE(C21,E21,J21),0)</f>
         <v>1</v>
       </c>
-      <c r="L21" s="0" t="str">
+      <c r="L21" s="4" t="str">
         <f aca="false">IF(K21&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -2861,7 +2850,7 @@
         <f aca="false">ROUND(AVERAGE(C22,E22,J22),0)</f>
         <v>10</v>
       </c>
-      <c r="L22" s="0" t="str">
+      <c r="L22" s="4" t="str">
         <f aca="false">IF(K22&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -2894,7 +2883,7 @@
         <f aca="false">ROUND(AVERAGE(C23,E23,J23),0)</f>
         <v>11</v>
       </c>
-      <c r="L23" s="0" t="str">
+      <c r="L23" s="4" t="str">
         <f aca="false">IF(K23&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -2915,18 +2904,18 @@
       <c r="G24" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="I24" s="0" t="n">
-        <v>9</v>
+      <c r="I24" s="5" t="n">
+        <v>17</v>
       </c>
       <c r="J24" s="0" t="n">
         <f aca="false">G24+I24/2</f>
-        <v>14.5</v>
+        <v>18.5</v>
       </c>
       <c r="K24" s="3" t="n">
         <f aca="false">ROUND(AVERAGE(C24,E24,J24),0)</f>
-        <v>11</v>
-      </c>
-      <c r="L24" s="0" t="str">
+        <v>13</v>
+      </c>
+      <c r="L24" s="4" t="str">
         <f aca="false">IF(K24&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -2947,7 +2936,7 @@
       <c r="G25" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="I25" s="0" t="n">
+      <c r="I25" s="5" t="n">
         <v>31</v>
       </c>
       <c r="J25" s="0" t="n">
@@ -2958,7 +2947,7 @@
         <f aca="false">ROUND(AVERAGE(C25,E25,J25),0)</f>
         <v>14</v>
       </c>
-      <c r="L25" s="0" t="str">
+      <c r="L25" s="4" t="str">
         <f aca="false">IF(K25&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -2990,7 +2979,7 @@
         <f aca="false">ROUND(AVERAGE(C26,E26,J26),0)</f>
         <v>13</v>
       </c>
-      <c r="L26" s="0" t="str">
+      <c r="L26" s="4" t="str">
         <f aca="false">IF(K26&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -3022,7 +3011,7 @@
         <f aca="false">ROUND(AVERAGE(C27,E27,J27),0)</f>
         <v>5</v>
       </c>
-      <c r="L27" s="0" t="str">
+      <c r="L27" s="4" t="str">
         <f aca="false">IF(K27&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -3059,7 +3048,7 @@
       <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.40234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.83"/>
@@ -3926,7 +3915,7 @@
       <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.38671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.40234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="18.83"/>
   </cols>
@@ -4592,7 +4581,7 @@
       <selection pane="topLeft" activeCell="I29" activeCellId="0" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.38671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.40234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="18.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.95"/>
@@ -5203,10 +5192,10 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.19"/>
   </cols>
   <sheetData>
@@ -5352,10 +5341,10 @@
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.19"/>
   </cols>
   <sheetData>
@@ -5536,10 +5525,10 @@
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.11"/>
   </cols>
@@ -5724,7 +5713,7 @@
       <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>